<commit_message>
Return only one movie for each director
</commit_message>
<xml_diff>
--- a/MovieDatabaseProcess/output-spreadsheets/movie-information.xlsx
+++ b/MovieDatabaseProcess/output-spreadsheets/movie-information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maggi\Documents\GitHub\rpa-solution\MovieDatabaseProcess\output-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFEDD4C-EC4B-40BB-BA18-9705C0A668F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302D4B14-972E-41ED-B905-8A029E09B047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12915" yWindow="2550" windowWidth="11400" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13260" yWindow="2895" windowWidth="11400" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Director</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Steven Spielberg</t>
+  </si>
+  <si>
+    <t>taika waititi</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,6 +377,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>